<commit_message>
Fix issues #20 and #21
</commit_message>
<xml_diff>
--- a/docassemble/LRFGuideMe/data/sources/HousingGuide_es.xlsx
+++ b/docassemble/LRFGuideMe/data/sources/HousingGuide_es.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="394">
   <si>
     <t xml:space="preserve">interview</t>
   </si>
@@ -2194,9 +2194,6 @@
   </si>
   <si>
     <t xml:space="preserve">agreement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acuerdo</t>
   </si>
   <si>
     <t xml:space="preserve">0a05317a6496bade15a34671b1ea1a73</t>
@@ -3271,11 +3268,11 @@
   </sheetPr>
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H110" activeCellId="0" sqref="H110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.72"/>
@@ -6118,7 +6115,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
         <v>8</v>
       </c>
@@ -6141,7 +6138,7 @@
         <v>281</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6155,19 +6152,19 @@
         <v>20</v>
       </c>
       <c r="D111" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111" s="5" t="s">
-        <v>284</v>
-      </c>
       <c r="H111" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6181,19 +6178,19 @@
         <v>21</v>
       </c>
       <c r="D112" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>286</v>
-      </c>
       <c r="H112" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6201,25 +6198,25 @@
         <v>8</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C113" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D113" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>289</v>
-      </c>
       <c r="H113" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6227,25 +6224,25 @@
         <v>8</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C114" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D114" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="5" t="s">
-        <v>291</v>
-      </c>
       <c r="H114" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6253,25 +6250,25 @@
         <v>8</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C115" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D115" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G115" s="3" t="s">
+      <c r="H115" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="H115" s="3" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6279,25 +6276,25 @@
         <v>8</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C116" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D116" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G116" s="5" t="s">
-        <v>296</v>
-      </c>
       <c r="H116" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6305,25 +6302,25 @@
         <v>8</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C117" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D117" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G117" s="5" t="s">
-        <v>298</v>
-      </c>
       <c r="H117" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6331,25 +6328,25 @@
         <v>8</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C118" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D118" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G118" s="5" t="s">
-        <v>300</v>
-      </c>
       <c r="H118" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6357,25 +6354,25 @@
         <v>8</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C119" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D119" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E119" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>303</v>
-      </c>
       <c r="H119" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6383,25 +6380,25 @@
         <v>8</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C120" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D120" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G120" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G120" s="5" t="s">
-        <v>305</v>
-      </c>
       <c r="H120" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6409,25 +6406,25 @@
         <v>8</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C121" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D121" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G121" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E121" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G121" s="3" t="s">
+      <c r="H121" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="H121" s="3" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6435,25 +6432,25 @@
         <v>8</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C122" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D122" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G122" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="E122" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G122" s="3" t="s">
+      <c r="H122" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="H122" s="3" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6461,25 +6458,25 @@
         <v>8</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C123" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D123" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G123" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="E123" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G123" s="5" t="s">
-        <v>313</v>
-      </c>
       <c r="H123" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6487,25 +6484,25 @@
         <v>8</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C124" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D124" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G124" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="E124" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G124" s="5" t="s">
-        <v>315</v>
-      </c>
       <c r="H124" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6513,25 +6510,25 @@
         <v>8</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C125" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D125" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G125" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G125" s="5" t="s">
-        <v>317</v>
-      </c>
       <c r="H125" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6539,25 +6536,25 @@
         <v>8</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C126" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D126" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G126" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="E126" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G126" s="5" t="s">
-        <v>319</v>
-      </c>
       <c r="H126" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6565,25 +6562,25 @@
         <v>8</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C127" s="2" t="n">
         <v>8</v>
       </c>
       <c r="D127" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G127" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="E127" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G127" s="5" t="s">
-        <v>321</v>
-      </c>
       <c r="H127" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6591,25 +6588,25 @@
         <v>8</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C128" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D128" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G128" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="E128" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G128" s="5" t="s">
-        <v>323</v>
-      </c>
       <c r="H128" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6617,25 +6614,25 @@
         <v>8</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C129" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D129" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G129" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E129" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G129" s="3" t="s">
+      <c r="H129" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="H129" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6643,25 +6640,25 @@
         <v>8</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C130" s="2" t="n">
         <v>11</v>
       </c>
       <c r="D130" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G130" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="E130" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F130" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G130" s="3" t="s">
-        <v>328</v>
-      </c>
       <c r="H130" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6669,25 +6666,25 @@
         <v>8</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C131" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D131" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G131" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E131" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G131" s="3" t="s">
+      <c r="H131" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="H131" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6695,25 +6692,25 @@
         <v>8</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C132" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D132" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G132" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E132" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G132" s="3" t="s">
+      <c r="H132" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="H132" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6721,25 +6718,25 @@
         <v>8</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C133" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D133" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G133" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="E133" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G133" s="3" t="s">
-        <v>337</v>
-      </c>
       <c r="H133" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6747,25 +6744,25 @@
         <v>8</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C134" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D134" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G134" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="E134" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G134" s="3" t="s">
+      <c r="H134" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="H134" s="3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6773,25 +6770,25 @@
         <v>8</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C135" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D135" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G135" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E135" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G135" s="3" t="s">
-        <v>342</v>
-      </c>
       <c r="H135" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6799,25 +6796,25 @@
         <v>8</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C136" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D136" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G136" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="E136" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>344</v>
-      </c>
       <c r="H136" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6825,25 +6822,25 @@
         <v>8</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C137" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D137" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G137" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="E137" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G137" s="3" t="s">
+      <c r="H137" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="H137" s="3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6851,25 +6848,25 @@
         <v>8</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C138" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D138" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G138" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="E138" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G138" s="3" t="s">
+      <c r="H138" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="H138" s="3" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6877,25 +6874,25 @@
         <v>8</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C139" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D139" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G139" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="E139" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F139" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G139" s="3" t="s">
+      <c r="H139" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="H139" s="3" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6903,25 +6900,25 @@
         <v>8</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C140" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D140" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G140" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="E140" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G140" s="3" t="s">
+      <c r="H140" s="3" t="s">
         <v>356</v>
-      </c>
-      <c r="H140" s="3" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6929,25 +6926,25 @@
         <v>8</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C141" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D141" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G141" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="E141" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G141" s="3" t="s">
+      <c r="H141" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="H141" s="3" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6955,25 +6952,25 @@
         <v>8</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C142" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G142" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="E142" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G142" s="3" t="s">
+      <c r="H142" s="3" t="s">
         <v>362</v>
-      </c>
-      <c r="H142" s="3" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6981,25 +6978,25 @@
         <v>8</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C143" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D143" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G143" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E143" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G143" s="3" t="s">
-        <v>366</v>
-      </c>
       <c r="H143" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7007,25 +7004,25 @@
         <v>8</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C144" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D144" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G144" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="E144" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G144" s="5" t="s">
+      <c r="H144" s="5" t="s">
         <v>368</v>
-      </c>
-      <c r="H144" s="5" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="172" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7033,25 +7030,25 @@
         <v>8</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C145" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D145" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G145" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="E145" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F145" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G145" s="3" t="s">
+      <c r="H145" s="7" t="s">
         <v>371</v>
-      </c>
-      <c r="H145" s="7" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7059,25 +7056,25 @@
         <v>8</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C146" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D146" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G146" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="E146" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F146" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G146" s="3" t="s">
-        <v>375</v>
-      </c>
       <c r="H146" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7085,25 +7082,25 @@
         <v>8</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C147" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D147" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G147" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="E147" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G147" s="3" t="s">
+      <c r="H147" s="8" t="s">
         <v>377</v>
-      </c>
-      <c r="H147" s="8" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7111,25 +7108,25 @@
         <v>8</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C148" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D148" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G148" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="E148" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F148" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G148" s="3" t="s">
-        <v>381</v>
-      </c>
       <c r="H148" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7137,25 +7134,25 @@
         <v>8</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C149" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D149" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G149" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="E149" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F149" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G149" s="3" t="s">
+      <c r="H149" s="3" t="s">
         <v>383</v>
-      </c>
-      <c r="H149" s="3" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7163,25 +7160,25 @@
         <v>8</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C150" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D150" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G150" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="E150" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F150" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G150" s="3" t="s">
+      <c r="H150" s="3" t="s">
         <v>386</v>
-      </c>
-      <c r="H150" s="3" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7189,25 +7186,25 @@
         <v>8</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C151" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D151" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G151" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="E151" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F151" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G151" s="3" t="s">
+      <c r="H151" s="8" t="s">
         <v>390</v>
-      </c>
-      <c r="H151" s="8" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7215,25 +7212,25 @@
         <v>8</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C152" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D152" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G152" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="E152" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F152" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G152" s="3" t="s">
+      <c r="H152" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="H152" s="3" t="s">
-        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>